<commit_message>
Add Beacon Driver components
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,24 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\Projects\Melty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B39B39D-D1C8-4598-B264-2A939D3D8CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413CD4B7-014A-4BDC-BDC4-992020CDF715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Oreo PCB" sheetId="1" r:id="rId1"/>
-    <sheet name="Mechanical" sheetId="2" r:id="rId2"/>
-    <sheet name="Calculator" sheetId="3" r:id="rId3"/>
+    <sheet name="Beacon Driver" sheetId="5" r:id="rId2"/>
+    <sheet name="Mechanical" sheetId="2" r:id="rId3"/>
+    <sheet name="Calculator" sheetId="3" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Beacon Driver'!$A$1:$I$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Oreo PCB'!$A$1:$I$28</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="186">
   <si>
     <t>Ref</t>
   </si>
@@ -395,9 +399,6 @@
     <t>HDPE</t>
   </si>
   <si>
-    <t>c2835 880kv BLDC</t>
-  </si>
-  <si>
     <t>1100mah 4s LiPo</t>
   </si>
   <si>
@@ -434,9 +435,6 @@
     <t>https://www.hobbyrc.co.uk/gnb-1100mah-4s-130c-lipo-battery</t>
   </si>
   <si>
-    <t>https://www.rclife.co.uk/Brushless-Motors/Surpass-Hobby-C2836-880kv-Brushless-Outrunner-Motor</t>
-  </si>
-  <si>
     <t>Density</t>
   </si>
   <si>
@@ -464,9 +462,6 @@
     <t>250g softner</t>
   </si>
   <si>
-    <t>IR LED</t>
-  </si>
-  <si>
     <t>https://www.digikey.co.uk/en/products/detail/osram-opto-ams-osram/LZ1-10R702-0000/4976715</t>
   </si>
   <si>
@@ -543,6 +538,66 @@
   </si>
   <si>
     <t>di</t>
+  </si>
+  <si>
+    <t>AL8860MP-13</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>LED Driver, 1 Output, Buck (Step Down), 4.5 V to 40 V in, 1 MHz switch, PWM, 40V/1.5 A out, MSOP-8</t>
+  </si>
+  <si>
+    <t>MSOP-8</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>VLS6045EX-470M-H</t>
+  </si>
+  <si>
+    <t>Power Inductor (SMD), AEC-Q200, 47 µH, 1.3 A, Semishielded, 1.8 A, VLS-EX-H</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>ES2AA</t>
+  </si>
+  <si>
+    <t>Fast / Ultrafast Diode, 50 V, 2 A, Single, 920 mV, 25 ns, 50 A</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>MFLA0805R1000FA</t>
+  </si>
+  <si>
+    <t>SMD Current Sense Resistor, 0.1 ohm, MFLA Series, 0805 [2012 Metric], 250 mW, ± 1%, Metal Film</t>
+  </si>
+  <si>
+    <t>LZ1-10R702-0000</t>
+  </si>
+  <si>
+    <t>Infrared (IR) Emitter 940nm 3V 1.2A 90° Star Array</t>
+  </si>
+  <si>
+    <t>Star Array</t>
+  </si>
+  <si>
+    <t>https://uk.farnell.com/diodes-inc/es2aa/diode-rectif-s-fast-2a-50v-sma/dp/2061427</t>
+  </si>
+  <si>
+    <t>SMA?</t>
+  </si>
+  <si>
+    <t>https://uk.farnell.com/tdk/vls6045ex-470m-h/inductor-aec-q200-47uh-semi-shld/dp/3288287</t>
   </si>
 </sst>
 </file>
@@ -555,7 +610,7 @@
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="&quot;£&quot;#,##0.000;[Red]\-&quot;£&quot;#,##0.000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -706,8 +761,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="40">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -901,12 +976,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFA9A9A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -914,12 +983,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1182,7 +1245,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1205,59 +1268,105 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="42" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="36" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="36" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="42" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
+    <xf numFmtId="164" fontId="18" fillId="35" borderId="0" xfId="42" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="42" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="18" fillId="36" borderId="0" xfId="42" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="8" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="42" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="42" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="20" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="20" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="20" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="20" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="20" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="42" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1621,18 +1730,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" customWidth="1"/>
     <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.44140625" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.77734375" customWidth="1"/>
     <col min="7" max="7" width="10.77734375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="92.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.44140625" style="61" customWidth="1"/>
+    <col min="9" max="9" width="45.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1643,7 +1755,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
@@ -1657,68 +1769,68 @@
       <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="53" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47" t="s">
+    <row r="2" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="47">
+      <c r="C2" s="38">
         <v>1</v>
       </c>
-      <c r="D2" s="48">
+      <c r="D2" s="39">
         <v>2</v>
       </c>
-      <c r="E2" s="49">
+      <c r="E2" s="40">
         <v>11.91</v>
       </c>
-      <c r="F2" s="47" t="s">
+      <c r="F2" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="50" t="s">
+      <c r="G2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="51" t="s">
+      <c r="H2" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="47" t="s">
+      <c r="I2" s="38" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="47" t="s">
+    <row r="3" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="38">
         <v>7</v>
       </c>
-      <c r="D3" s="48">
+      <c r="D3" s="39">
         <v>20</v>
       </c>
-      <c r="E3" s="52">
+      <c r="E3" s="43">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="H3" s="51" t="s">
+      <c r="H3" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="38" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1742,7 +1854,7 @@
       <c r="G4" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="55">
         <v>100</v>
       </c>
     </row>
@@ -1766,33 +1878,33 @@
       <c r="G5" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="55">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="47" t="s">
+    <row r="6" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="38">
         <v>7</v>
       </c>
-      <c r="D6" s="48">
+      <c r="D6" s="39">
         <v>20</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E6" s="43">
         <v>0.11</v>
       </c>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="50">
+      <c r="G6" s="41">
         <v>1206</v>
       </c>
-      <c r="H6" s="47" t="s">
+      <c r="H6" s="56" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1816,7 +1928,7 @@
       <c r="G7" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="55">
         <v>100</v>
       </c>
     </row>
@@ -1840,7 +1952,7 @@
       <c r="G8" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="55">
         <v>20</v>
       </c>
     </row>
@@ -1864,7 +1976,7 @@
       <c r="G9" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="55">
         <v>200</v>
       </c>
     </row>
@@ -1886,7 +1998,7 @@
       <c r="G10" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="55">
         <v>50</v>
       </c>
     </row>
@@ -1908,36 +2020,36 @@
       <c r="G11" s="4">
         <v>1210</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="55">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="53" t="s">
+    <row r="12" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="53">
+      <c r="C12" s="38">
         <v>12</v>
       </c>
-      <c r="D12" s="54">
+      <c r="D12" s="39">
         <v>24</v>
       </c>
-      <c r="E12" s="55">
+      <c r="E12" s="43">
         <v>0.371</v>
       </c>
-      <c r="F12" s="53" t="s">
+      <c r="F12" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="56" t="s">
+      <c r="G12" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="57" t="s">
+      <c r="H12" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="I12" s="53" t="s">
+      <c r="I12" s="38" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1961,7 +2073,7 @@
       <c r="G13" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="55">
         <v>200</v>
       </c>
     </row>
@@ -1983,7 +2095,7 @@
       <c r="G14" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="55">
         <v>50</v>
       </c>
     </row>
@@ -2007,88 +2119,88 @@
       <c r="G15" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="55">
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="53" t="s">
+    <row r="16" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="53">
+      <c r="C16" s="38">
         <v>12</v>
       </c>
-      <c r="D16" s="54">
+      <c r="D16" s="39">
         <v>24</v>
       </c>
-      <c r="E16" s="55">
+      <c r="E16" s="43">
         <v>0.17299999999999999</v>
       </c>
-      <c r="F16" s="53" t="s">
+      <c r="F16" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="56" t="s">
+      <c r="G16" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="H16" s="53" t="s">
+      <c r="H16" s="56" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+    <row r="17" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="38">
         <v>1</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="39">
         <v>3</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="43">
         <v>0.37</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="G17" s="28" t="s">
+      <c r="G17" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="H17" s="26" t="s">
+      <c r="H17" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="I17" s="26" t="s">
+      <c r="I17" s="38" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="62" t="s">
+    <row r="18" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="62">
+      <c r="C18" s="44">
         <v>2</v>
       </c>
-      <c r="D18" s="63">
+      <c r="D18" s="45">
         <v>10</v>
       </c>
-      <c r="E18" s="64">
+      <c r="E18" s="46">
         <v>0.38</v>
       </c>
-      <c r="F18" s="62" t="s">
+      <c r="F18" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="65" t="s">
+      <c r="G18" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="H18" s="62" t="s">
+      <c r="H18" s="57" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2112,36 +2224,36 @@
       <c r="G19" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="55">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="53" t="s">
+    <row r="20" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="53" t="s">
+      <c r="B20" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="53">
+      <c r="C20" s="38">
         <v>2</v>
       </c>
-      <c r="D20" s="54">
+      <c r="D20" s="39">
         <v>5</v>
       </c>
-      <c r="E20" s="55">
+      <c r="E20" s="43">
         <v>1.4</v>
       </c>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="G20" s="56" t="s">
+      <c r="G20" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="H20" s="53" t="s">
+      <c r="H20" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="I20" s="53" t="s">
+      <c r="I20" s="38" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2165,7 +2277,7 @@
       <c r="G21" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="55">
         <v>10</v>
       </c>
     </row>
@@ -2187,33 +2299,33 @@
       <c r="G22" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H22" s="58">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="26" t="s">
+    <row r="23" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="38">
         <v>4</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D23" s="39">
         <v>8</v>
       </c>
-      <c r="E23" s="30">
+      <c r="E23" s="43">
         <v>0.18</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="G23" s="28" t="s">
+      <c r="G23" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="26" t="s">
+      <c r="H23" s="56" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2232,74 +2344,75 @@
       <c r="G24" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H24" s="20" t="s">
+      <c r="H24" s="55" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="47" t="s">
+    <row r="25" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="47">
+      <c r="C25" s="38">
         <v>2</v>
       </c>
-      <c r="D25" s="48">
+      <c r="D25" s="39">
         <v>10</v>
       </c>
-      <c r="E25" s="52">
+      <c r="E25" s="43">
         <v>0.64</v>
       </c>
-      <c r="F25" s="47" t="s">
+      <c r="F25" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="G25" s="50"/>
-      <c r="H25" s="51" t="s">
+      <c r="G25" s="41"/>
+      <c r="H25" s="54" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="58" t="s">
+    <row r="26" spans="1:9" s="49" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="B26" s="58" t="s">
+      <c r="B26" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="C26" s="58">
+      <c r="C26" s="49">
         <v>2</v>
       </c>
-      <c r="D26" s="59">
+      <c r="D26" s="50">
         <v>5</v>
       </c>
-      <c r="E26" s="60">
+      <c r="E26" s="51">
         <v>0.43</v>
       </c>
-      <c r="F26" s="58" t="s">
+      <c r="F26" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="G26" s="61" t="s">
+      <c r="G26" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="H26" s="58" t="s">
+      <c r="H26" s="59" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="31" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="31" t="s">
+    <row r="27" spans="1:9" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="C27" s="31">
+      <c r="C27" s="24">
         <v>1</v>
       </c>
-      <c r="D27" s="32">
+      <c r="D27" s="25">
         <v>5</v>
       </c>
-      <c r="E27" s="33">
+      <c r="E27" s="26">
         <v>5</v>
       </c>
-      <c r="G27" s="34"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="60"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
@@ -2315,6 +2428,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I28" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="H25" r:id="rId1" xr:uid="{17CB87F0-57F2-4564-AFCC-207D0A2CB847}"/>
     <hyperlink ref="H2" r:id="rId2" xr:uid="{A666E5CD-24D2-4C68-861D-FC284E2E0CA9}"/>
@@ -2327,11 +2441,226 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65E3385-B438-413B-8224-CBB11CA591CC}">
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" style="76" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" style="76" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="76" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" style="76" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="76" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.77734375" style="76" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" style="78" customWidth="1"/>
+    <col min="8" max="8" width="43.44140625" style="79" customWidth="1"/>
+    <col min="9" max="9" width="45.109375" style="76" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="76"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="73" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="73" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="73" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="68" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="68" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="68" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="68">
+        <v>1</v>
+      </c>
+      <c r="D2" s="69">
+        <v>4</v>
+      </c>
+      <c r="E2" s="85">
+        <v>0.73</v>
+      </c>
+      <c r="F2" s="68" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="86"/>
+    </row>
+    <row r="3" spans="1:9" s="68" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="68" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="68">
+        <v>1</v>
+      </c>
+      <c r="D3" s="69">
+        <v>3</v>
+      </c>
+      <c r="E3" s="70">
+        <v>0.36</v>
+      </c>
+      <c r="F3" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" s="71" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="86" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="68" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="68" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" s="68" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="68">
+        <v>1</v>
+      </c>
+      <c r="D4" s="69">
+        <v>5</v>
+      </c>
+      <c r="E4" s="70">
+        <v>0.08</v>
+      </c>
+      <c r="F4" s="68" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" s="71" t="s">
+        <v>184</v>
+      </c>
+      <c r="H4" s="72" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="68" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="68" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" s="68" t="s">
+        <v>178</v>
+      </c>
+      <c r="C5" s="68">
+        <v>1</v>
+      </c>
+      <c r="D5" s="69">
+        <v>10</v>
+      </c>
+      <c r="E5" s="70">
+        <v>0.09</v>
+      </c>
+      <c r="F5" s="68" t="s">
+        <v>179</v>
+      </c>
+      <c r="G5" s="71" t="s">
+        <v>108</v>
+      </c>
+      <c r="H5" s="72"/>
+    </row>
+    <row r="6" spans="1:9" s="64" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="64" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="64" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" s="64">
+        <v>1</v>
+      </c>
+      <c r="D6" s="65">
+        <v>2</v>
+      </c>
+      <c r="E6" s="67">
+        <v>8.33</v>
+      </c>
+      <c r="F6" s="64" t="s">
+        <v>181</v>
+      </c>
+      <c r="G6" s="66" t="s">
+        <v>182</v>
+      </c>
+      <c r="H6" s="42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="80" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="80" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="80">
+        <v>1</v>
+      </c>
+      <c r="D7" s="81">
+        <v>5</v>
+      </c>
+      <c r="E7" s="82">
+        <v>3</v>
+      </c>
+      <c r="G7" s="83"/>
+      <c r="H7" s="84"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="76" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="77">
+        <f>SUMPRODUCT(C2:C7,E2:E7)</f>
+        <v>12.59</v>
+      </c>
+      <c r="D8" s="77">
+        <f>SUMPRODUCT(D2:D7,E2:E7)</f>
+        <v>36.96</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H6" r:id="rId1" xr:uid="{4F6839DA-111B-4CF0-87AC-DDDBFFA545BB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2363,127 +2692,127 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="C2" s="26">
+    <row r="2" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="22">
         <v>318419</v>
       </c>
-      <c r="D2" s="26">
+      <c r="D2" s="22">
         <f>C2*$J$7*0.5</f>
         <v>159.20949999999999</v>
       </c>
-      <c r="E2" s="26">
+      <c r="E2" s="22">
         <v>1</v>
       </c>
-      <c r="F2" s="38"/>
-      <c r="I2" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="J2" s="42"/>
-    </row>
-    <row r="3" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="C3" s="26">
+      <c r="F2" s="29"/>
+      <c r="I2" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="J2" s="33"/>
+    </row>
+    <row r="3" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="22">
         <v>838261</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="22">
         <f>C3*$J$7*0.5</f>
         <v>419.13049999999998</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="22">
         <v>1</v>
       </c>
-      <c r="F3" s="38"/>
-      <c r="I3" s="43" t="s">
+      <c r="F3" s="29"/>
+      <c r="I3" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="J3" s="44">
+      <c r="J3" s="35">
         <f>0.95/10^3</f>
         <v>9.5E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>165</v>
-      </c>
-      <c r="C4" s="26">
+    <row r="4" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="22">
         <v>59807.32</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="22">
         <f>C4*J6</f>
         <v>468.88938880000001</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="22">
         <v>0</v>
       </c>
-      <c r="F4" s="38"/>
-      <c r="I4" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="J4" s="44">
+      <c r="F4" s="29"/>
+      <c r="I4" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="J4" s="35">
         <f>1/10^3</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="C5" s="26">
+    <row r="5" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="22">
         <v>72054.759999999995</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="22">
         <f>J6*C5</f>
         <v>564.90931839999996</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="22">
         <v>0</v>
       </c>
-      <c r="F5" s="38"/>
-      <c r="I5" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="J5" s="44">
+      <c r="F5" s="29"/>
+      <c r="I5" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="J5" s="35">
         <f>2.7/10^3</f>
         <v>2.7000000000000001E-3</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I6" s="43" t="s">
+      <c r="I6" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="J6" s="44">
+      <c r="J6" s="35">
         <f>7.84/10^3</f>
         <v>7.8399999999999997E-3</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I7" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="J7" s="46">
+      <c r="I7" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="J7" s="37">
         <v>1E-3</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B8">
         <v>550</v>
@@ -2498,7 +2827,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B9">
         <v>700</v>
@@ -2521,10 +2850,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C11">
         <v>2000</v>
@@ -2539,10 +2868,10 @@
     </row>
     <row r="12" spans="1:10" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C12" s="8">
         <v>5000</v>
@@ -2558,7 +2887,7 @@
     </row>
     <row r="13" spans="1:10" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>11</v>
@@ -2573,200 +2902,169 @@
     </row>
     <row r="14" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="D14" s="22">
+        <v>65</v>
+      </c>
+      <c r="E14" s="22">
+        <v>2</v>
+      </c>
+      <c r="F14" s="29">
+        <v>18.43</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G15" s="21"/>
+    </row>
+    <row r="16" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="D14" s="22">
-        <v>67</v>
-      </c>
-      <c r="E14" s="22">
-        <v>0</v>
-      </c>
-      <c r="F14" s="23">
-        <v>13.99</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="D15" s="26">
-        <v>65</v>
-      </c>
-      <c r="E15" s="26">
-        <v>2</v>
-      </c>
-      <c r="F15" s="38">
-        <v>18.43</v>
-      </c>
-      <c r="G15" s="29" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G16" s="25"/>
-    </row>
-    <row r="17" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="47" t="s">
-        <v>120</v>
-      </c>
-      <c r="D17" s="47">
+      <c r="D16" s="38">
         <v>137</v>
       </c>
-      <c r="E17" s="47">
+      <c r="E16" s="38">
         <v>1</v>
       </c>
-      <c r="F17" s="66">
+      <c r="F16" s="48">
         <v>18.55</v>
       </c>
-      <c r="G17" s="47" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="47" t="s">
-        <v>128</v>
-      </c>
-      <c r="E18" s="47">
+      <c r="G16" s="38" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="E17" s="38">
         <v>1</v>
       </c>
-      <c r="F18" s="66">
+      <c r="F17" s="48">
         <f>'Oreo PCB'!C28</f>
         <v>36.045200000000008</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>129</v>
-      </c>
-      <c r="E19">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18">
         <v>1</v>
       </c>
-      <c r="F19" s="13"/>
+      <c r="F18" s="13"/>
+    </row>
+    <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="3">
+        <v>5</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="14"/>
     </row>
     <row r="20" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D20" s="3">
-        <v>5</v>
-      </c>
       <c r="E20" s="3">
         <v>1</v>
       </c>
       <c r="F20" s="14"/>
     </row>
-    <row r="21" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:7" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="8">
         <v>1</v>
       </c>
-      <c r="F21" s="14"/>
-    </row>
-    <row r="22" spans="1:7" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E22" s="8">
+      <c r="F21" s="15"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="62" t="s">
+        <v>134</v>
+      </c>
+      <c r="C22" s="62"/>
+      <c r="D22" s="16">
+        <f>SUMPRODUCT(D2:D21,E2:E21)</f>
+        <v>1565.2199999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="63" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="63"/>
+      <c r="D23">
+        <f>1500-D22</f>
+        <v>-65.2199999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="20"/>
+    </row>
+    <row r="27" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="E27" s="38">
         <v>1</v>
       </c>
-      <c r="F22" s="15"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="36" t="s">
+      <c r="F27" s="48">
+        <v>24</v>
+      </c>
+      <c r="G27" s="42" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="E28" s="38">
+        <v>1</v>
+      </c>
+      <c r="F28" s="48">
+        <v>25</v>
+      </c>
+      <c r="G28" s="42" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="16">
-        <f>SUMPRODUCT(D2:D22,E2:E22)</f>
-        <v>1565.2199999999998</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="37" t="s">
+      <c r="E29" s="22">
+        <v>1</v>
+      </c>
+      <c r="F29" s="29">
+        <v>4.99</v>
+      </c>
+      <c r="G29" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24">
-        <f>1500-D23</f>
-        <v>-65.2199999999998</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="21"/>
-    </row>
-    <row r="28" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="47" t="s">
-        <v>144</v>
-      </c>
-      <c r="E28" s="47">
-        <v>1</v>
-      </c>
-      <c r="F28" s="66">
-        <v>24</v>
-      </c>
-      <c r="G28" s="51" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="E29" s="47">
-        <v>1</v>
-      </c>
-      <c r="F29" s="66">
-        <v>25</v>
-      </c>
-      <c r="G29" s="51" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="E30" s="26">
-        <v>1</v>
-      </c>
-      <c r="F30" s="38">
-        <v>4.99</v>
-      </c>
-      <c r="G30" s="39" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="47" t="s">
-        <v>142</v>
-      </c>
-      <c r="E31" s="47">
-        <v>2</v>
-      </c>
-      <c r="F31" s="66">
-        <v>8.5500000000000007</v>
-      </c>
-      <c r="G31" s="51" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G33" s="17"/>
-    </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G34" s="17"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G31" s="17"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G32" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="2">
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
   </mergeCells>
-  <conditionalFormatting sqref="D24">
+  <conditionalFormatting sqref="D23">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="-150"/>
@@ -2779,17 +3077,15 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G14" r:id="rId1" xr:uid="{03F112B5-B3B2-4909-8BD4-1E98727497CC}"/>
-    <hyperlink ref="G28" r:id="rId2" xr:uid="{5762EC35-6A2B-48B3-A0AC-25547F451DAD}"/>
-    <hyperlink ref="G29" r:id="rId3" xr:uid="{1C18DF23-300D-473C-9EAD-17A994FDB54A}"/>
-    <hyperlink ref="G31" r:id="rId4" xr:uid="{125A4910-4799-4ED0-ADC1-E040E57AC6FA}"/>
-    <hyperlink ref="G30" r:id="rId5" xr:uid="{1FF79E27-4DF4-4DD3-9675-B842CADB7A9D}"/>
+    <hyperlink ref="G27" r:id="rId1" xr:uid="{5762EC35-6A2B-48B3-A0AC-25547F451DAD}"/>
+    <hyperlink ref="G28" r:id="rId2" xr:uid="{1C18DF23-300D-473C-9EAD-17A994FDB54A}"/>
+    <hyperlink ref="G29" r:id="rId3" xr:uid="{1FF79E27-4DF4-4DD3-9675-B842CADB7A9D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7BCE403-71D1-49A7-B189-9C894C701DB1}">
   <dimension ref="B2:H18"/>
   <sheetViews>
@@ -2803,19 +3099,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="40" t="s">
-        <v>157</v>
+      <c r="B2" s="31" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E3" t="s">
         <v>113</v>
@@ -2824,7 +3120,7 @@
         <v>114</v>
       </c>
       <c r="G3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
@@ -2856,19 +3152,19 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="40" t="s">
-        <v>161</v>
+      <c r="B7" s="31" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E8" t="s">
         <v>113</v>
@@ -2878,11 +3174,11 @@
       <c r="B9">
         <v>20</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="28">
         <f>C4</f>
         <v>35</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="28">
         <f>50</f>
         <v>50</v>
       </c>
@@ -2908,8 +3204,8 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="40" t="s">
-        <v>166</v>
+      <c r="B14" s="31" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
@@ -2936,10 +3232,10 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C16" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Separate BOM for each PCB
Add separate BOM for the Main Board, IR Board, and IR Beacon
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\Projects\Melty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413CD4B7-014A-4BDC-BDC4-992020CDF715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E200636-4F37-43A0-8476-456D594ADAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Oreo PCB" sheetId="1" r:id="rId1"/>
-    <sheet name="Beacon Driver" sheetId="5" r:id="rId2"/>
-    <sheet name="Mechanical" sheetId="2" r:id="rId3"/>
-    <sheet name="Calculator" sheetId="3" r:id="rId4"/>
+    <sheet name="Main Board BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="IR Board BOM" sheetId="6" r:id="rId2"/>
+    <sheet name="IR Beacon BOM" sheetId="5" r:id="rId3"/>
+    <sheet name="Mechanical" sheetId="2" r:id="rId4"/>
+    <sheet name="Calculator" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Beacon Driver'!$A$1:$I$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Oreo PCB'!$A$1:$I$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'IR Beacon BOM'!$A$1:$I$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'IR Board BOM'!$A$1:$I$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Main Board BOM'!$A$1:$I$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="201">
   <si>
     <t>Ref</t>
   </si>
@@ -327,15 +329,6 @@
     <t>https://www.digikey.co.uk/en/products/detail/harvatek-corporation/B3803FCH-20C001112U1930/13588742</t>
   </si>
   <si>
-    <t>D3, D4,</t>
-  </si>
-  <si>
-    <t>3mm / 5mm THT LED</t>
-  </si>
-  <si>
-    <t>LED THT 3mm / 5mm</t>
-  </si>
-  <si>
     <t>Q1,</t>
   </si>
   <si>
@@ -561,9 +554,6 @@
     <t>Power Inductor (SMD), AEC-Q200, 47 µH, 1.3 A, Semishielded, 1.8 A, VLS-EX-H</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
     <t>ES2AA</t>
   </si>
   <si>
@@ -598,6 +588,63 @@
   </si>
   <si>
     <t>https://uk.farnell.com/tdk/vls6045ex-470m-h/inductor-aec-q200-47uh-semi-shld/dp/3288287</t>
+  </si>
+  <si>
+    <t>https://fr.farnell.com/en-FR/eaton-bussmann/mfla0805r1000fa/res-r1-1-0-25w-metal-film-0805/dp/4070738</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Slide-Switches_Yuandi-TA-3539S-A1_C514054.html</t>
+  </si>
+  <si>
+    <t>TA-3539S-A1</t>
+  </si>
+  <si>
+    <t>https://uk.farnell.com/diodes-inc/al8860mp-13/led-driver-buck-1mhz-msop-8/dp/2709526</t>
+  </si>
+  <si>
+    <t>SMD,4x7.2mm Slide Switche</t>
+  </si>
+  <si>
+    <t>https://www.lcsc.com/product-detail/Infrared-IR-LEDs_XSSY-SE03-EMC3838A-C90-940_C5205231.html</t>
+  </si>
+  <si>
+    <t>D0x</t>
+  </si>
+  <si>
+    <t>D1x</t>
+  </si>
+  <si>
+    <t>SE03-EMC3838A-C90-940</t>
+  </si>
+  <si>
+    <t>180mW~240mW 1000mA 1.3V~1.7V 1.7W 930nm~960nm SMD,3.9x3.9mm Infrared (IR) LED</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2004181005_Yuandi-TA-3539S-A1_C514054.pdf</t>
+  </si>
+  <si>
+    <t>Supplier Link</t>
+  </si>
+  <si>
+    <t>https://www.farnell.com/datasheets/2875164.pdf</t>
+  </si>
+  <si>
+    <t>https://www.farnell.com/datasheets/2211370.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>2 units needed</t>
+  </si>
+  <si>
+    <t>https://uk.farnell.com/stmicroelectronics/std80n3ll/mosfet-n-ch-30v-80a-to-252/dp/4036303?CMP=KNC-GUK-GEN-KWL-RLSA-PUR-TEST-921&amp;mckv=_dc|pcrid|610187768070|&amp;gclid=Cj0KCQjwz8emBhDrARIsANNJjS6BriV4xIs_x6XmtyKd7ZRa-XmyrBPjHKZbWgFfGnDnOGN-Ei2ZlYcaAudcEALw_wcB</t>
+  </si>
+  <si>
+    <t>STD80N3LL</t>
   </si>
 </sst>
 </file>
@@ -610,7 +657,7 @@
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="&quot;£&quot;#,##0.000;[Red]\-&quot;£&quot;#,##0.000"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -768,13 +815,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -988,7 +1028,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1245,7 +1285,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1266,66 +1306,57 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="42" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="36" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="36" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="18" fillId="35" borderId="0" xfId="42" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="8" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="42" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="20" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="20" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="20" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="42" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1334,39 +1365,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="20" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="20" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="20" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="20" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="8" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="20" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="42" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1728,10 +1797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1739,11 +1808,11 @@
     <col min="1" max="1" width="6.6640625" customWidth="1"/>
     <col min="2" max="2" width="27.109375" customWidth="1"/>
     <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" style="36" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="54.77734375" customWidth="1"/>
     <col min="7" max="7" width="10.77734375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="43.44140625" style="61" customWidth="1"/>
+    <col min="8" max="8" width="20.21875" style="35" customWidth="1"/>
     <col min="9" max="9" width="45.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1755,9 +1824,9 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="D1" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="32" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -1769,68 +1838,66 @@
       <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="53" t="s">
-        <v>6</v>
+      <c r="H1" s="32" t="s">
+        <v>194</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
+    <row r="2" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="38">
-        <v>1</v>
-      </c>
-      <c r="D2" s="39">
+      <c r="C2" s="61">
+        <v>1</v>
+      </c>
+      <c r="D2" s="86">
         <v>2</v>
       </c>
-      <c r="E2" s="40">
+      <c r="E2" s="72">
         <v>11.91</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="54" t="s">
+      <c r="G2" s="64"/>
+      <c r="H2" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="I2" s="61" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+    <row r="3" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="61">
         <v>7</v>
       </c>
-      <c r="D3" s="39">
+      <c r="D3" s="86">
         <v>20</v>
       </c>
-      <c r="E3" s="43">
+      <c r="E3" s="63">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="H3" s="54" t="s">
+      <c r="G3" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="38" t="s">
+      <c r="I3" s="61" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1844,7 +1911,9 @@
       <c r="C4" s="3">
         <v>2</v>
       </c>
-      <c r="D4" s="18"/>
+      <c r="D4" s="81">
+        <v>100</v>
+      </c>
       <c r="E4" s="10">
         <v>1.1999999999999999E-3</v>
       </c>
@@ -1852,10 +1921,13 @@
         <v>21</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="H4" s="55">
+        <v>106</v>
+      </c>
+      <c r="H4" s="33">
         <v>100</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1868,7 +1940,9 @@
       <c r="C5" s="3">
         <v>4</v>
       </c>
-      <c r="D5" s="18"/>
+      <c r="D5" s="81">
+        <v>50</v>
+      </c>
       <c r="E5" s="10">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -1876,36 +1950,42 @@
         <v>24</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="H5" s="55">
+        <v>106</v>
+      </c>
+      <c r="H5" s="33">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="I5" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="61">
         <v>7</v>
       </c>
-      <c r="D6" s="39">
+      <c r="D6" s="86">
         <v>20</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="63">
         <v>0.11</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="41">
+      <c r="G6" s="64">
         <v>1206</v>
       </c>
-      <c r="H6" s="56" t="s">
+      <c r="H6" s="65" t="s">
         <v>28</v>
+      </c>
+      <c r="I6" s="61" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1918,7 +1998,9 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="18"/>
+      <c r="D7" s="82">
+        <v>100</v>
+      </c>
       <c r="E7" s="10">
         <v>8.0000000000000004E-4</v>
       </c>
@@ -1926,10 +2008,13 @@
         <v>31</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="H7" s="55">
+        <v>106</v>
+      </c>
+      <c r="H7" s="33">
         <v>100</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1942,7 +2027,9 @@
       <c r="C8" s="3">
         <v>1</v>
       </c>
-      <c r="D8" s="18"/>
+      <c r="D8" s="82">
+        <v>20</v>
+      </c>
       <c r="E8" s="10">
         <v>1.9199999999999998E-2</v>
       </c>
@@ -1950,10 +2037,13 @@
         <v>34</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="H8" s="55">
+        <v>107</v>
+      </c>
+      <c r="H8" s="33">
         <v>20</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1966,7 +2056,9 @@
       <c r="C9" s="3">
         <v>5</v>
       </c>
-      <c r="D9" s="18"/>
+      <c r="D9" s="82">
+        <v>200</v>
+      </c>
       <c r="E9" s="10">
         <v>8.0000000000000004E-4</v>
       </c>
@@ -1974,10 +2066,13 @@
         <v>37</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="H9" s="55">
+        <v>106</v>
+      </c>
+      <c r="H9" s="33">
         <v>200</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1990,16 +2085,21 @@
       <c r="C10" s="3">
         <v>1</v>
       </c>
-      <c r="D10" s="18"/>
+      <c r="D10" s="82">
+        <v>50</v>
+      </c>
       <c r="E10" s="10"/>
       <c r="F10" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="H10" s="55">
+        <v>107</v>
+      </c>
+      <c r="H10" s="33">
         <v>50</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2012,7 +2112,9 @@
       <c r="C11" s="3">
         <v>1</v>
       </c>
-      <c r="D11" s="18"/>
+      <c r="D11" s="82">
+        <v>10</v>
+      </c>
       <c r="E11" s="10"/>
       <c r="F11" s="3" t="s">
         <v>43</v>
@@ -2020,635 +2122,570 @@
       <c r="G11" s="4">
         <v>1210</v>
       </c>
-      <c r="H11" s="55">
+      <c r="H11" s="33">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="38" t="s">
+      <c r="I11" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="61" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" s="61">
+        <v>12</v>
+      </c>
+      <c r="D12" s="88"/>
+      <c r="E12" s="63"/>
+      <c r="G12" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="65" t="s">
+        <v>199</v>
+      </c>
+      <c r="I12" s="61" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="73" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="38">
+      <c r="C13" s="73">
         <v>12</v>
       </c>
-      <c r="D12" s="39">
+      <c r="D13" s="85">
         <v>24</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E13" s="74">
         <v>0.371</v>
       </c>
-      <c r="F12" s="38" t="s">
+      <c r="F13" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="41" t="s">
+      <c r="G13" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="54" t="s">
+      <c r="H13" s="89" t="s">
         <v>48</v>
       </c>
-      <c r="I12" s="38" t="s">
+      <c r="I13" s="73" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="3">
-        <v>8</v>
-      </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="10">
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="H13" s="55">
-        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C14" s="3">
-        <v>1</v>
-      </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="10"/>
+        <v>8</v>
+      </c>
+      <c r="D14" s="82">
+        <v>200</v>
+      </c>
+      <c r="E14" s="10">
+        <v>4.0000000000000002E-4</v>
+      </c>
       <c r="F14" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H14" s="55">
-        <v>50</v>
+        <v>106</v>
+      </c>
+      <c r="H14" s="33">
+        <v>200</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="82">
+        <v>50</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H15" s="33">
+        <v>50</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C16" s="3">
         <v>7</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="10">
+      <c r="D16" s="82">
+        <v>200</v>
+      </c>
+      <c r="E16" s="10">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="H15" s="55">
+      <c r="G16" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H16" s="33">
         <v>200</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="38" t="s">
+      <c r="I16" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B17" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="38">
+      <c r="C17" s="61">
         <v>12</v>
       </c>
-      <c r="D16" s="39">
+      <c r="D17" s="86">
         <v>24</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E17" s="63">
         <v>0.17299999999999999</v>
       </c>
-      <c r="F16" s="38" t="s">
+      <c r="F17" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="H16" s="56" t="s">
+      <c r="G17" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="H17" s="65" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="38" t="s">
+      <c r="I17" s="61" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B18" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="38">
-        <v>1</v>
-      </c>
-      <c r="D17" s="39">
+      <c r="C18" s="61">
+        <v>1</v>
+      </c>
+      <c r="D18" s="86">
         <v>3</v>
       </c>
-      <c r="E17" s="43">
+      <c r="E18" s="63">
         <v>0.37</v>
       </c>
-      <c r="F17" s="38" t="s">
+      <c r="F18" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="G17" s="41" t="s">
+      <c r="G18" s="64" t="s">
         <v>65</v>
       </c>
-      <c r="H17" s="56" t="s">
+      <c r="H18" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="I17" s="38" t="s">
+      <c r="I18" s="61" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="44" t="s">
+    <row r="19" spans="1:9" s="73" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B19" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="44">
+      <c r="C19" s="73">
+        <v>0</v>
+      </c>
+      <c r="D19" s="85">
+        <v>10</v>
+      </c>
+      <c r="E19" s="74">
+        <v>0.38</v>
+      </c>
+      <c r="F19" s="73" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19" s="75" t="s">
+        <v>71</v>
+      </c>
+      <c r="H19" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" s="73" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="81">
+        <v>10</v>
+      </c>
+      <c r="E20" s="10">
+        <v>4.5</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H20" s="33">
+        <v>10</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="61">
         <v>2</v>
       </c>
-      <c r="D18" s="45">
+      <c r="D21" s="86">
+        <v>5</v>
+      </c>
+      <c r="E21" s="63">
+        <v>1.4</v>
+      </c>
+      <c r="F21" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="H21" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="I21" s="61" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1</v>
+      </c>
+      <c r="D22" s="81">
         <v>10</v>
       </c>
-      <c r="E18" s="46">
-        <v>0.38</v>
-      </c>
-      <c r="F18" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="H18" s="57" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="3">
-        <v>1</v>
-      </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="10">
-        <v>4.5</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H19" s="55">
+      <c r="E22" s="10">
+        <v>0.1017</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H22" s="33">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" s="38">
-        <v>2</v>
-      </c>
-      <c r="D20" s="39">
-        <v>5</v>
-      </c>
-      <c r="E20" s="43">
-        <v>1.4</v>
-      </c>
-      <c r="F20" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="G20" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="H20" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="I20" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C21" s="3">
-        <v>1</v>
-      </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="10">
-        <v>0.1017</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="H21" s="55">
+      <c r="I22" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="8">
+        <v>1</v>
+      </c>
+      <c r="D23" s="83">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C22" s="8">
-        <v>1</v>
-      </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="8" t="s">
+      <c r="E23" s="11"/>
+      <c r="F23" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G23" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="H22" s="58">
+      <c r="H23" s="34">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="B23" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23" s="38">
-        <v>4</v>
-      </c>
-      <c r="D23" s="39">
-        <v>8</v>
-      </c>
-      <c r="E23" s="43">
-        <v>0.18</v>
-      </c>
-      <c r="F23" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="G23" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" s="56" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C24" s="3">
-        <v>4</v>
-      </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="H24" s="55" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="C25" s="38">
-        <v>2</v>
-      </c>
-      <c r="D25" s="39">
+      <c r="I23" s="8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="68" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="68">
+        <v>1</v>
+      </c>
+      <c r="D24" s="87">
         <v>10</v>
       </c>
-      <c r="E25" s="43">
-        <v>0.64</v>
-      </c>
-      <c r="F25" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="G25" s="41"/>
-      <c r="H25" s="54" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="49" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="49" t="s">
-        <v>102</v>
-      </c>
-      <c r="B26" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" s="49">
-        <v>2</v>
-      </c>
-      <c r="D26" s="50">
-        <v>5</v>
-      </c>
-      <c r="E26" s="51">
-        <v>0.43</v>
-      </c>
-      <c r="F26" s="49" t="s">
+      <c r="E24" s="69">
+        <v>0.4</v>
+      </c>
+      <c r="G24" s="70"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="68" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
         <v>104</v>
       </c>
-      <c r="G26" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" s="59" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" s="24">
-        <v>1</v>
-      </c>
-      <c r="D27" s="25">
-        <v>5</v>
-      </c>
-      <c r="E27" s="26">
-        <v>5</v>
-      </c>
-      <c r="G27" s="27"/>
-      <c r="H27" s="60"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>107</v>
-      </c>
-      <c r="C28" s="1">
-        <f>SUMPRODUCT(C2:C27,E2:E27)</f>
-        <v>36.045200000000008</v>
-      </c>
-      <c r="D28" s="1">
-        <f>SUMPRODUCT(D2:D27,E2:E27)</f>
-        <v>87.115999999999985</v>
+      <c r="C25" s="1">
+        <f>SUMPRODUCT(C2:C24,E2:E24)</f>
+        <v>27.825200000000002</v>
+      </c>
+      <c r="D25" s="84">
+        <f>SUMPRODUCT(D2:D24,E2:E24)</f>
+        <v>103.25699999999999</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I28" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I25" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="H25" r:id="rId1" xr:uid="{17CB87F0-57F2-4564-AFCC-207D0A2CB847}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{A666E5CD-24D2-4C68-861D-FC284E2E0CA9}"/>
-    <hyperlink ref="H3" r:id="rId3" xr:uid="{CDDEC637-0CC2-4C8E-BD21-C096A986417B}"/>
-    <hyperlink ref="H12" r:id="rId4" xr:uid="{968F9FCF-FA36-415F-B39F-7A92308C2335}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{A666E5CD-24D2-4C68-861D-FC284E2E0CA9}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{CDDEC637-0CC2-4C8E-BD21-C096A986417B}"/>
+    <hyperlink ref="H13" r:id="rId3" xr:uid="{968F9FCF-FA36-415F-B39F-7A92308C2335}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65E3385-B438-413B-8224-CBB11CA591CC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ED2662A-9FE1-4A7E-AC46-2D55231AEE5C}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="76" customWidth="1"/>
-    <col min="2" max="2" width="27.109375" style="76" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" style="76" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5546875" style="76" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="76" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.77734375" style="76" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" style="78" customWidth="1"/>
-    <col min="8" max="8" width="43.44140625" style="79" customWidth="1"/>
-    <col min="9" max="9" width="45.109375" style="76" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="76"/>
+    <col min="1" max="1" width="6.6640625" style="61" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" style="61" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="61" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" style="61" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="61" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.77734375" style="61" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" style="64" customWidth="1"/>
+    <col min="8" max="8" width="20.21875" style="65" customWidth="1"/>
+    <col min="9" max="9" width="45.109375" style="61" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="61"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="73" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="73" t="s">
+    <row r="1" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="73" t="s">
-        <v>143</v>
-      </c>
-      <c r="D1" s="73" t="s">
+      <c r="B1" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="E1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="73" t="s">
+      <c r="F1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="74" t="s">
+      <c r="G1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="75" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="73" t="s">
+      <c r="H1" s="60" t="s">
+        <v>194</v>
+      </c>
+      <c r="I1" s="58" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="68" t="s">
-        <v>167</v>
-      </c>
-      <c r="B2" s="68" t="s">
-        <v>166</v>
-      </c>
-      <c r="C2" s="68">
-        <v>1</v>
-      </c>
-      <c r="D2" s="69">
-        <v>4</v>
-      </c>
-      <c r="E2" s="85">
-        <v>0.73</v>
-      </c>
-      <c r="F2" s="68" t="s">
-        <v>168</v>
-      </c>
-      <c r="G2" s="71" t="s">
-        <v>169</v>
-      </c>
-      <c r="H2" s="86"/>
-    </row>
-    <row r="3" spans="1:9" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="68" t="s">
-        <v>170</v>
-      </c>
-      <c r="B3" s="68" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3" s="68">
-        <v>1</v>
-      </c>
-      <c r="D3" s="69">
-        <v>3</v>
-      </c>
-      <c r="E3" s="70">
-        <v>0.36</v>
-      </c>
-      <c r="F3" s="68" t="s">
-        <v>172</v>
-      </c>
-      <c r="G3" s="71" t="s">
+    <row r="2" spans="1:9" s="73" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="73" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="73" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="73">
+        <v>0</v>
+      </c>
+      <c r="D2" s="77">
+        <v>8</v>
+      </c>
+      <c r="E2" s="74">
+        <v>0.18</v>
+      </c>
+      <c r="F2" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="86" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="68" t="s">
-        <v>177</v>
-      </c>
-      <c r="B4" s="68" t="s">
-        <v>174</v>
-      </c>
-      <c r="C4" s="68">
-        <v>1</v>
-      </c>
-      <c r="D4" s="69">
+      <c r="H2" s="76" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="73" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="61" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="61" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="61">
+        <v>1</v>
+      </c>
+      <c r="D3" s="78">
+        <v>10</v>
+      </c>
+      <c r="E3" s="63">
+        <v>0.64</v>
+      </c>
+      <c r="F3" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" s="66" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" s="61" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="58" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="58">
+        <v>1</v>
+      </c>
+      <c r="D4" s="79">
         <v>5</v>
       </c>
-      <c r="E4" s="70">
-        <v>0.08</v>
-      </c>
-      <c r="F4" s="68" t="s">
-        <v>175</v>
-      </c>
-      <c r="G4" s="71" t="s">
-        <v>184</v>
-      </c>
-      <c r="H4" s="72" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="68" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="68" t="s">
-        <v>176</v>
-      </c>
+      <c r="E4" s="67">
+        <v>0.43</v>
+      </c>
+      <c r="F4" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="I4" s="58" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="68" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="68" t="s">
-        <v>178</v>
+        <v>103</v>
       </c>
       <c r="C5" s="68">
         <v>1</v>
       </c>
-      <c r="D5" s="69">
-        <v>10</v>
-      </c>
-      <c r="E5" s="70">
-        <v>0.09</v>
-      </c>
-      <c r="F5" s="68" t="s">
-        <v>179</v>
-      </c>
-      <c r="G5" s="71" t="s">
-        <v>108</v>
-      </c>
-      <c r="H5" s="72"/>
-    </row>
-    <row r="6" spans="1:9" s="64" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="64" t="s">
-        <v>173</v>
-      </c>
-      <c r="B6" s="64" t="s">
-        <v>180</v>
-      </c>
-      <c r="C6" s="64">
-        <v>1</v>
-      </c>
-      <c r="D6" s="65">
-        <v>2</v>
-      </c>
-      <c r="E6" s="67">
-        <v>8.33</v>
-      </c>
-      <c r="F6" s="64" t="s">
-        <v>181</v>
-      </c>
-      <c r="G6" s="66" t="s">
-        <v>182</v>
-      </c>
-      <c r="H6" s="42" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="80" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="80" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="80">
-        <v>1</v>
-      </c>
-      <c r="D7" s="81">
+      <c r="D5" s="80">
         <v>5</v>
       </c>
-      <c r="E7" s="82">
-        <v>3</v>
-      </c>
-      <c r="G7" s="83"/>
-      <c r="H7" s="84"/>
+      <c r="E5" s="69">
+        <v>0.4</v>
+      </c>
+      <c r="G5" s="70"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="68" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="61" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="72">
+        <f>SUMPRODUCT(C2:C5,E2:E5)</f>
+        <v>1.4700000000000002</v>
+      </c>
+      <c r="D6" s="72">
+        <f>SUMPRODUCT(D2:D5,E2:E5)</f>
+        <v>11.99</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="76" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="77">
-        <f>SUMPRODUCT(C2:C7,E2:E7)</f>
-        <v>12.59</v>
-      </c>
-      <c r="D8" s="77">
-        <f>SUMPRODUCT(D2:D7,E2:E7)</f>
-        <v>36.96</v>
+      <c r="B8" s="62" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I6" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="H6" r:id="rId1" xr:uid="{4F6839DA-111B-4CF0-87AC-DDDBFFA545BB}"/>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{30458312-C6E3-4D8A-BC7B-EFDECBD0FD33}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2656,11 +2693,305 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65E3385-B438-413B-8224-CBB11CA591CC}">
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" style="43" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" style="43" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" style="43" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="43" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.77734375" style="43" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" style="45" customWidth="1"/>
+    <col min="8" max="8" width="22" style="46" customWidth="1"/>
+    <col min="9" max="9" width="45.109375" style="43" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="43"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="40" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="37">
+        <v>1</v>
+      </c>
+      <c r="D2" s="37">
+        <v>4</v>
+      </c>
+      <c r="E2" s="51">
+        <v>0.73</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" s="52" t="s">
+        <v>186</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="37">
+        <v>1</v>
+      </c>
+      <c r="D3" s="37">
+        <v>3</v>
+      </c>
+      <c r="E3" s="38">
+        <v>0.36</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="G3" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="52" t="s">
+        <v>181</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="37">
+        <v>1</v>
+      </c>
+      <c r="D4" s="37">
+        <v>5</v>
+      </c>
+      <c r="E4" s="38">
+        <v>0.08</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="H4" s="55" t="s">
+        <v>179</v>
+      </c>
+      <c r="I4" s="37" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="56">
+        <v>1</v>
+      </c>
+      <c r="D5" s="37">
+        <v>10</v>
+      </c>
+      <c r="E5" s="38">
+        <v>0.09</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="55" t="s">
+        <v>182</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="C6" s="37">
+        <v>1</v>
+      </c>
+      <c r="D6" s="37">
+        <v>2</v>
+      </c>
+      <c r="E6" s="38">
+        <v>8.33</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="H6" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="I6" s="37" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" s="37">
+        <v>1</v>
+      </c>
+      <c r="D7" s="37">
+        <v>3</v>
+      </c>
+      <c r="E7" s="38">
+        <v>1.58</v>
+      </c>
+      <c r="F7" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="G7" s="39"/>
+      <c r="H7" s="57" t="s">
+        <v>188</v>
+      </c>
+      <c r="I7" s="37" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="37" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="C8" s="37">
+        <v>1</v>
+      </c>
+      <c r="D8" s="37">
+        <v>10</v>
+      </c>
+      <c r="E8" s="38">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="G8" s="39"/>
+      <c r="H8" s="57" t="s">
+        <v>184</v>
+      </c>
+      <c r="I8" s="37" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="47" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="47">
+        <v>1</v>
+      </c>
+      <c r="D9" s="47">
+        <v>5</v>
+      </c>
+      <c r="E9" s="48">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="G9" s="49"/>
+      <c r="H9" s="50"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="44">
+        <f>SUMPRODUCT(C2:C9,E2:E9)</f>
+        <v>12.071000000000002</v>
+      </c>
+      <c r="D10" s="44">
+        <f>SUMPRODUCT(D2:D9,E2:E9)</f>
+        <v>31.710000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F22" s="17"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H6" r:id="rId1" xr:uid="{4F6839DA-111B-4CF0-87AC-DDDBFFA545BB}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{0366DFD5-AAEF-4C9D-88CA-919633823A6B}"/>
+    <hyperlink ref="H5" r:id="rId3" xr:uid="{E8F791BD-9C8E-44FF-B5A0-16877BC669C9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2671,148 +3002,148 @@
   <sheetData>
     <row r="1" spans="1:10" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>115</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="C2" s="22">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="61" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="61">
         <v>318419</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2" s="61">
         <f>C2*$J$7*0.5</f>
         <v>159.20949999999999</v>
       </c>
-      <c r="E2" s="22">
-        <v>1</v>
-      </c>
-      <c r="F2" s="29"/>
-      <c r="I2" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="J2" s="33"/>
-    </row>
-    <row r="3" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="C3" s="22">
+      <c r="E2" s="61">
+        <v>1</v>
+      </c>
+      <c r="F2" s="90"/>
+      <c r="I2" s="92" t="s">
+        <v>128</v>
+      </c>
+      <c r="J2" s="93"/>
+    </row>
+    <row r="3" spans="1:10" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="61" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="61" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="61">
         <v>838261</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="61">
         <f>C3*$J$7*0.5</f>
         <v>419.13049999999998</v>
       </c>
-      <c r="E3" s="22">
-        <v>1</v>
-      </c>
-      <c r="F3" s="29"/>
-      <c r="I3" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="J3" s="35">
+      <c r="E3" s="61">
+        <v>1</v>
+      </c>
+      <c r="F3" s="90"/>
+      <c r="I3" s="94" t="s">
+        <v>115</v>
+      </c>
+      <c r="J3" s="95">
         <f>0.95/10^3</f>
         <v>9.5E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="C4" s="22">
+    <row r="4" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="20">
         <v>59807.32</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="20">
         <f>C4*J6</f>
         <v>468.88938880000001</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="20">
         <v>0</v>
       </c>
-      <c r="F4" s="29"/>
-      <c r="I4" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="J4" s="35">
+      <c r="F4" s="23"/>
+      <c r="I4" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" s="27">
         <f>1/10^3</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="C5" s="22">
+    <row r="5" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="20">
         <v>72054.759999999995</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="20">
         <f>J6*C5</f>
         <v>564.90931839999996</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="20">
         <v>0</v>
       </c>
-      <c r="F5" s="29"/>
-      <c r="I5" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="J5" s="35">
+      <c r="F5" s="23"/>
+      <c r="I5" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="J5" s="27">
         <f>2.7/10^3</f>
         <v>2.7000000000000001E-3</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I6" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="J6" s="35">
+      <c r="I6" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="J6" s="27">
         <f>7.84/10^3</f>
         <v>7.8399999999999997E-3</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I7" s="36" t="s">
-        <v>133</v>
-      </c>
-      <c r="J7" s="37">
+      <c r="I7" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="J7" s="29">
         <v>1E-3</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B8">
         <v>550</v>
@@ -2827,7 +3158,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B9">
         <v>700</v>
@@ -2850,10 +3181,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C11">
         <v>2000</v>
@@ -2866,28 +3197,28 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="C12" s="8">
+    <row r="12" spans="1:10" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="58" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="58" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="58">
         <v>5000</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="58">
         <f>C12*$J$4</f>
         <v>5</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="58">
         <v>2</v>
       </c>
-      <c r="F12" s="15"/>
+      <c r="F12" s="91"/>
     </row>
     <row r="13" spans="1:10" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>11</v>
@@ -2900,58 +3231,58 @@
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="D14" s="22">
+    <row r="14" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" s="20">
         <v>65</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="20">
         <v>2</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="23">
         <v>18.43</v>
       </c>
-      <c r="G14" s="23" t="s">
-        <v>144</v>
+      <c r="G14" s="21" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G15" s="21"/>
-    </row>
-    <row r="16" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="D16" s="38">
+      <c r="G15" s="19"/>
+    </row>
+    <row r="16" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="30">
         <v>137</v>
       </c>
-      <c r="E16" s="38">
-        <v>1</v>
-      </c>
-      <c r="F16" s="48">
+      <c r="E16" s="30">
+        <v>1</v>
+      </c>
+      <c r="F16" s="31">
         <v>18.55</v>
       </c>
-      <c r="G16" s="38" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="38" t="s">
+      <c r="G16" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="E17" s="38">
-        <v>1</v>
-      </c>
-      <c r="F17" s="48">
-        <f>'Oreo PCB'!C28</f>
-        <v>36.045200000000008</v>
+    </row>
+    <row r="17" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" s="30">
+        <v>1</v>
+      </c>
+      <c r="F17" s="31">
+        <f>'Main Board BOM'!C25</f>
+        <v>27.825200000000002</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -2960,7 +3291,7 @@
     </row>
     <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D19" s="3">
         <v>5</v>
@@ -2972,7 +3303,7 @@
     </row>
     <row r="20" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E20" s="3">
         <v>1</v>
@@ -2981,7 +3312,7 @@
     </row>
     <row r="21" spans="1:7" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E21" s="8">
         <v>1</v>
@@ -2989,68 +3320,68 @@
       <c r="F21" s="15"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="62" t="s">
-        <v>134</v>
-      </c>
-      <c r="C22" s="62"/>
+      <c r="B22" s="53" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22" s="53"/>
       <c r="D22" s="16">
         <f>SUMPRODUCT(D2:D21,E2:E21)</f>
         <v>1565.2199999999998</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="63" t="s">
-        <v>135</v>
-      </c>
-      <c r="C23" s="63"/>
+      <c r="B23" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" s="54"/>
       <c r="D23">
         <f>1500-D22</f>
         <v>-65.2199999999998</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
-    </row>
-    <row r="27" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="38" t="s">
-        <v>141</v>
-      </c>
-      <c r="E27" s="38">
-        <v>1</v>
-      </c>
-      <c r="F27" s="48">
+      <c r="A25" s="18"/>
+    </row>
+    <row r="27" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="61" t="s">
+        <v>138</v>
+      </c>
+      <c r="E27" s="61">
+        <v>1</v>
+      </c>
+      <c r="F27" s="90">
         <v>24</v>
       </c>
-      <c r="G27" s="42" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="38" t="s">
+      <c r="G27" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="E28" s="38">
-        <v>1</v>
-      </c>
-      <c r="F28" s="48">
+    </row>
+    <row r="28" spans="1:7" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="61" t="s">
+        <v>136</v>
+      </c>
+      <c r="E28" s="61">
+        <v>1</v>
+      </c>
+      <c r="F28" s="90">
         <v>25</v>
       </c>
-      <c r="G28" s="42" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="E29" s="22">
-        <v>1</v>
-      </c>
-      <c r="F29" s="29">
+      <c r="G28" s="19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="E29" s="20">
+        <v>1</v>
+      </c>
+      <c r="F29" s="23">
         <v>4.99</v>
       </c>
-      <c r="G29" s="30" t="s">
-        <v>137</v>
+      <c r="G29" s="24" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -3085,7 +3416,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7BCE403-71D1-49A7-B189-9C894C701DB1}">
   <dimension ref="B2:H18"/>
   <sheetViews>
@@ -3099,28 +3430,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="31" t="s">
-        <v>154</v>
+      <c r="B2" s="25" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
@@ -3152,33 +3483,33 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="31" t="s">
-        <v>158</v>
+      <c r="B7" s="25" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>20</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="22">
         <f>C4</f>
         <v>35</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="22">
         <f>50</f>
         <v>50</v>
       </c>
@@ -3204,8 +3535,8 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="31" t="s">
-        <v>163</v>
+      <c r="B14" s="25" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
@@ -3232,10 +3563,10 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">

</xml_diff>